<commit_message>
v2p7. Multibody on CRG roads (R2022a and higher), OpenCRG 1.1.2, MF-Swift 2022.1, geometry fix for Mac
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Tire/MFMbody/sm_car_data_Tire_MFMbody.xlsx
+++ b/Libraries/Vehicle/Tire/MFMbody/sm_car_data_Tire_MFMbody.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Tire\MFMbody\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Tire\MFMbody\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D41C6E-30A2-4E45-B560-ACBD70644AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D38A93D-B997-47B4-9449-09EE6C5BCFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3444" yWindow="1452" windowWidth="17280" windowHeight="14232" tabRatio="840" activeTab="5" xr2:uid="{038AE485-2DF6-4480-A05B-AFF15F06FE64}"/>
+    <workbookView xWindow="5925" yWindow="2310" windowWidth="21600" windowHeight="11385" tabRatio="840" xr2:uid="{038AE485-2DF6-4480-A05B-AFF15F06FE64}"/>
   </bookViews>
   <sheets>
     <sheet name="Tir_235_50R24" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="29">
   <si>
     <t>Units</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>MFMbody_235_50R24</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>fContactPoint</t>
+  </si>
+  <si>
+    <t>Break algebraic loop between tire center position and contact point position and orientation</t>
   </si>
 </sst>
 </file>
@@ -782,22 +794,22 @@
   </sheetPr>
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="10" width="6.6640625" customWidth="1"/>
+    <col min="9" max="10" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -817,7 +829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -842,7 +854,7 @@
       <c r="T2"/>
       <c r="U2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -866,7 +878,7 @@
       <c r="T3"/>
       <c r="U3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -891,7 +903,7 @@
       <c r="T4"/>
       <c r="U4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -914,7 +926,7 @@
       <c r="T5"/>
       <c r="U5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -942,7 +954,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -973,75 +985,87 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="C15" s="17"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="C16" s="17"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="6"/>
       <c r="C19" s="17"/>
@@ -1057,7 +1081,7 @@
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="6"/>
       <c r="C20" s="17"/>
@@ -1075,22 +1099,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C15:C18 A15:A18 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8 A8">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1111,21 +1140,21 @@
       <selection activeCell="J10" sqref="J10"/>
       <selection pane="topRight" activeCell="J10" sqref="J10"/>
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6:G6"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="13" width="6.6640625" customWidth="1"/>
+    <col min="9" max="13" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1145,7 +1174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1174,7 +1203,7 @@
       <c r="X2"/>
       <c r="Y2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1201,7 +1230,7 @@
       <c r="X3"/>
       <c r="Y3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +1258,7 @@
       <c r="X4"/>
       <c r="Y4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1255,7 +1284,7 @@
       <c r="X5"/>
       <c r="Y5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1283,7 +1312,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1314,39 +1343,51 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="C9" s="17"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="C10" s="17"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="6"/>
       <c r="C13" s="17"/>
@@ -1366,7 +1407,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="6"/>
       <c r="C14" s="17"/>
@@ -1388,22 +1429,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C9:C12 A9:A12 C4:D5 A4:A5">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
     <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1423,21 +1474,21 @@
       <selection activeCell="J10" sqref="J10"/>
       <selection pane="topRight" activeCell="J10" sqref="J10"/>
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6:G6"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="13" width="6.6640625" customWidth="1"/>
+    <col min="9" max="13" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1457,7 +1508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1486,7 +1537,7 @@
       <c r="X2"/>
       <c r="Y2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1513,7 +1564,7 @@
       <c r="X3"/>
       <c r="Y3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1541,7 +1592,7 @@
       <c r="X4"/>
       <c r="Y4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1567,7 +1618,7 @@
       <c r="X5"/>
       <c r="Y5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1595,7 +1646,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1626,45 +1677,57 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="C10" s="17"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="C11" s="17"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="6"/>
       <c r="C14" s="17"/>
@@ -1684,7 +1747,7 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="6"/>
       <c r="C15" s="17"/>
@@ -1706,22 +1769,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10:C13 A10:A13 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1741,21 +1814,21 @@
       <selection activeCell="J10" sqref="J10"/>
       <selection pane="topRight" activeCell="J10" sqref="J10"/>
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6:G6"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="13" width="6.6640625" customWidth="1"/>
+    <col min="9" max="13" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1775,7 +1848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1804,7 +1877,7 @@
       <c r="X2"/>
       <c r="Y2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1831,7 +1904,7 @@
       <c r="X3"/>
       <c r="Y3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1859,7 +1932,7 @@
       <c r="X4"/>
       <c r="Y4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1885,7 +1958,7 @@
       <c r="X5"/>
       <c r="Y5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1913,7 +1986,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1944,39 +2017,51 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="C9" s="17"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="C10" s="17"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="6"/>
       <c r="C13" s="17"/>
@@ -1996,7 +2081,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="6"/>
       <c r="C14" s="17"/>
@@ -2018,22 +2103,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C9:C12 A9:A12 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2054,21 +2149,21 @@
       <selection activeCell="H30" sqref="H30"/>
       <selection pane="topRight" activeCell="H30" sqref="H30"/>
       <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6:G6"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="13" width="6.6640625" customWidth="1"/>
+    <col min="9" max="13" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2088,7 +2183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2117,7 +2212,7 @@
       <c r="X2"/>
       <c r="Y2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2144,7 +2239,7 @@
       <c r="X3"/>
       <c r="Y3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2172,7 +2267,7 @@
       <c r="X4"/>
       <c r="Y4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2198,7 +2293,7 @@
       <c r="X5"/>
       <c r="Y5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -2226,7 +2321,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2257,45 +2352,57 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="C10" s="17"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="C11" s="17"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="6"/>
       <c r="C14" s="17"/>
@@ -2315,7 +2422,7 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="6"/>
       <c r="C15" s="17"/>
@@ -2337,22 +2444,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10:C13 A10:A13 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2367,26 +2484,26 @@
   </sheetPr>
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C19" sqref="C19"/>
       <selection pane="topRight" activeCell="C19" sqref="C19"/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
-      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2406,7 +2523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2437,7 +2554,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2466,7 +2583,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2494,7 +2611,7 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2520,7 +2637,7 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -2548,7 +2665,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2579,11 +2696,23 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="H8" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
@@ -2602,7 +2731,7 @@
       <c r="Z8"/>
       <c r="AA8"/>
     </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -2619,7 +2748,7 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -2637,79 +2766,79 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="C17" s="17"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="C18" s="17"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="C21" s="17"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="C22" s="17"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -2719,7 +2848,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -2729,7 +2858,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -2743,7 +2872,7 @@
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -2758,18 +2887,28 @@
       <c r="T26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C17:C20 A17:A20 C4:D7 A4:A9 C8:C9">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="C17:C20 A17:A20 C4:D7 A4:A7 C9 A9">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
v2.9. Added default for roadFile to MFMBody.xlsx, Scrollable to UI.
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Tire/MFMbody/sm_car_data_Tire_MFMbody.xlsx
+++ b/Libraries/Vehicle/Tire/MFMbody/sm_car_data_Tire_MFMbody.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Tire\MFMbody\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Tire\MFMbody\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D38A93D-B997-47B4-9449-09EE6C5BCFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDF2E48-629A-47EF-9347-B4141BAC7F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="2310" windowWidth="21600" windowHeight="11385" tabRatio="840" xr2:uid="{038AE485-2DF6-4480-A05B-AFF15F06FE64}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11430" tabRatio="840" xr2:uid="{038AE485-2DF6-4480-A05B-AFF15F06FE64}"/>
   </bookViews>
   <sheets>
     <sheet name="Tir_235_50R24" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="31">
   <si>
     <t>Units</t>
   </si>
@@ -124,6 +124,12 @@
   <si>
     <t>Break algebraic loop between tire center position and contact point position and orientation</t>
   </si>
+  <si>
+    <t>roadFile</t>
+  </si>
+  <si>
+    <t>which('TNO_FlatRoad.rdf')</t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -236,11 +242,54 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -792,10 +841,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,27 +1036,35 @@
     </row>
     <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -1041,7 +1098,6 @@
     </row>
     <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
-      <c r="C15" s="17"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -1055,6 +1111,7 @@
     </row>
     <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
+      <c r="C17" s="17"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -1068,12 +1125,12 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="17"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="18"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -1097,29 +1154,44 @@
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
     </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="18"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C15:C18 A15:A18 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
+  <conditionalFormatting sqref="C16:C19 A16:A19 C4:D5 A4:A5">
+    <cfRule type="cellIs" dxfId="39" priority="7" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8 A8">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9 A9">
+    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8 C8:D8">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1133,14 +1205,14 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AA15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="J10" sqref="J10"/>
       <selection pane="topRight" activeCell="J10" sqref="J10"/>
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,28 +1417,35 @@
     </row>
     <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -1377,6 +1456,7 @@
     </row>
     <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
+      <c r="C11" s="17"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -1390,12 +1470,12 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="17"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="18"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -1427,34 +1507,49 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
     </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="18"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C9:C12 A9:A12 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+  <conditionalFormatting sqref="C10:C13 A10:A13 C4:D5 A4:A5">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8 C8:D8">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1467,14 +1562,14 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="J10" sqref="J10"/>
       <selection pane="topRight" activeCell="J10" sqref="J10"/>
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,27 +1774,398 @@
     </row>
     <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="20" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C11:C14 A11:A14 C4:D5 A4:A5">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D7 A6:A7">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8 C8:D8">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB49D6F-468E-418F-A062-1D81E654217C}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AA15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="J10" sqref="J10"/>
+      <selection pane="topRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="10" customWidth="1"/>
+    <col min="9" max="13" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+    </row>
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+    </row>
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+    </row>
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+    </row>
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <v>10</v>
+      </c>
+      <c r="J6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+    </row>
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="16">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+    </row>
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -1721,11 +2187,25 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
@@ -1756,65 +2236,61 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="18"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10:C13 A10:A13 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8 C8:D8">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB49D6F-468E-418F-A062-1D81E654217C}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFE2FD0-25ED-4314-9A75-8473D14A2B34}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="J10" sqref="J10"/>
-      <selection pane="topRight" activeCell="J10" sqref="J10"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection activeCell="H30" sqref="H30"/>
+      <selection pane="topRight" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,7 +2362,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -1940,7 +2416,7 @@
       <c r="C5" s="5"/>
       <c r="G5" s="13"/>
       <c r="H5" s="20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J5"/>
       <c r="L5"/>
@@ -2019,366 +2495,38 @@
     </row>
     <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C9:C12 A9:A12 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFE2FD0-25ED-4314-9A75-8473D14A2B34}">
-  <sheetPr>
-    <tabColor theme="3" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:AA15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="H30" sqref="H30"/>
-      <selection pane="topRight" activeCell="H30" sqref="H30"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="13" width="6.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2"/>
-    </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-    </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-    </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-    </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16">
-        <v>10</v>
-      </c>
-      <c r="J6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="16">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6">
-        <v>2</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-    </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="C10" s="17"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -2392,6 +2540,7 @@
     </row>
     <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
+      <c r="C12" s="17"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -2405,12 +2554,12 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="18"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -2442,34 +2591,49 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="18"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C10:C13 A10:A13 C4:D5 A4:A5">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+  <conditionalFormatting sqref="C11:C14 A11:A14 C4:D5 A4:A5">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D7 A6:A7">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8 C8:D8">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2489,7 +2653,7 @@
       <selection activeCell="C19" sqref="C19"/>
       <selection pane="topRight" activeCell="C19" sqref="C19"/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,20 +2862,16 @@
     </row>
     <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
-        <v>26</v>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23" t="s">
+        <v>30</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -2732,10 +2892,22 @@
       <c r="AA8"/>
     </row>
     <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -2750,9 +2922,9 @@
     </row>
     <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10" s="22"/>
@@ -2804,7 +2976,6 @@
     </row>
     <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
-      <c r="C17" s="17"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -2818,6 +2989,7 @@
     </row>
     <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
+      <c r="C19" s="17"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -2830,8 +3002,9 @@
     </row>
     <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="H21" s="18"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
@@ -2839,14 +3012,9 @@
       <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
+      <c r="A23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
@@ -2887,27 +3055,32 @@
       <c r="T26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C17:C20 A17:A20 C4:D7 A4:A7 C9 A9">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+  <conditionalFormatting sqref="C18:C21 A18:A21 C10 A10 C4:D7 A4:A7">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
-      <formula>"class"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8 C8:D8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>

</xml_diff>